<commit_message>
Erster test der Excel
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cornelius\Desktop\HISS PROJECT\wizard-of-oz\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhilippReinhard\Skripte\wizard-of-oz\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44BB3EC-7D1B-4E08-95BF-35D5FC201D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1C9F8B-9D03-4ACA-B743-750F8D3DFB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31068" yWindow="4992" windowWidth="14400" windowHeight="7272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openTickets" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>ticketCreator</t>
   </si>
@@ -89,9 +89,6 @@
     <t>[{"start":3, "end":6, "key":"Fehlerbeschreibung"},{"start":45, "end":60, "key":"System"}]</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -105,6 +102,21 @@
   </si>
   <si>
     <t>01.12.2022</t>
+  </si>
+  <si>
+    <t>John Lennon</t>
+  </si>
+  <si>
+    <t>05.01.2022</t>
+  </si>
+  <si>
+    <t>"Analysis for Excel" Add-In causes crashes</t>
+  </si>
+  <si>
+    <t>Hello, Is there any more stable version of "Analysis for Excel" for Office 365? This one causes a lot of crashes when run with VBA. My current version is as attached - 2.8.</t>
+  </si>
+  <si>
+    <t>[{"start":45, "end":60, "key":"Fehlerbeschreibung"},{"start":30, "end":45, "key":"System"}]</t>
   </si>
 </sst>
 </file>
@@ -140,10 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -522,22 +533,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="2" max="3" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="40.453125" customWidth="1"/>
+    <col min="6" max="6" width="131.36328125" customWidth="1"/>
+    <col min="7" max="7" width="83.6328125" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="11" width="13.140625" customWidth="1"/>
+    <col min="9" max="11" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -569,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <f t="shared" ref="A2:A5" si="0">IFERROR(A1+1,0)</f>
         <v>0</v>
@@ -602,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -611,19 +622,19 @@
         <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -635,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -644,10 +655,10 @@
         <v>345</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -668,7 +679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -677,10 +688,10 @@
         <v>567</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -701,8 +712,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
         <f>IFERROR(A5+1,0)</f>
         <v>4</v>
       </c>
@@ -710,13 +721,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
fixed problem with database (error was in config excel)
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhilippReinhard\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cornelius\Desktop\HISS PROJECT\wizard-of-oz\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBAEBFF-8F87-45A6-8999-AA160511549D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0727C8BA-AB56-4EA2-BE5B-CADEE4ADCBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openTickets" sheetId="1" r:id="rId1"/>
@@ -169,158 +169,122 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -335,15 +299,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}" name="Table2" displayName="Table2" ref="A1:J5" totalsRowShown="0">
   <autoFilter ref="A1:J5" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}"/>
   <tableColumns count="10">
-    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="20">
+    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(A1+1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{F788B06C-E20D-499B-82A2-16BDBA4E08F2}" name="ticketId"/>
@@ -626,21 +586,21 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="5" max="5" width="40.453125" customWidth="1"/>
-    <col min="6" max="6" width="131.453125" customWidth="1"/>
-    <col min="7" max="7" width="83.54296875" customWidth="1"/>
+    <col min="2" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="131.42578125" customWidth="1"/>
+    <col min="7" max="7" width="83.5703125" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="11" width="13.1796875" customWidth="1"/>
+    <col min="9" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -672,7 +632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A4" si="0">IFERROR(A1+1,0)</f>
         <v>0</v>
@@ -705,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -738,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -771,8 +731,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f>IFERROR(A4+1,0)</f>
         <v>3</v>
       </c>
@@ -804,13 +764,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0</v>
       </c>
@@ -839,84 +799,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A16:J16 A4:D4 G4:J4 A2:J3">
-    <cfRule type="containsBlanks" dxfId="10" priority="17">
+    <cfRule type="containsBlanks" dxfId="15" priority="17">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:J3">
-    <cfRule type="containsBlanks" dxfId="19" priority="16">
+    <cfRule type="containsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D4 G4:J4">
-    <cfRule type="containsBlanks" dxfId="18" priority="15">
+    <cfRule type="containsBlanks" dxfId="13" priority="15">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="16" priority="13">
+    <cfRule type="containsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsBlanks" dxfId="15" priority="12">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(D16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsBlanks" dxfId="14" priority="11">
+    <cfRule type="containsBlanks" dxfId="10" priority="11">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsBlanks" dxfId="12" priority="9">
+    <cfRule type="containsBlanks" dxfId="9" priority="9">
       <formula>LEN(TRIM(D16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="containsBlanks" dxfId="11" priority="8">
+    <cfRule type="containsBlanks" dxfId="8" priority="8">
       <formula>LEN(TRIM(F16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="7" priority="7">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(F2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:F5">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(D5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(D5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(D5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Uploaded new excel files
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cornelius\Desktop\HISS PROJECT\RB\wizard-of-oz\client\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wikassel-my.sharepoint.com/personal/mahei_li_wi-kassel_de/Documents/Crowdsupport/05 Publikationen/2023/DESRIST_Reference Process for Labeling/03_Data Experiment/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF08C376-65BE-4F83-A5FD-670FE634A835}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30936" yWindow="2640" windowWidth="30960" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openTickets" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={76F8C2AA-920B-4DF9-9FF9-807CFE50611C}</author>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{76F8C2AA-920B-4DF9-9FF9-807CFE50611C}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Hier Ende der Problembeschreobung weggelassen, da nicht verstanden, was gemeint ist.
+Original: Campus 1 : MY / Cisco soft phone unable to use
+2021-06-24 05:03:58 - Mas Azra Zabirah Mohd Azahari (Additional comments)
+Additional Location Information: 
+Affected Device: Cisco soft phone
+Issue description: Unable to use CISCO soft phone even though has been installed, set up and test by IT support team and no CISCO soft phone install in CITRIX in case  need to use the soft phone in the CITRIX window.
+Need soft phone issue to resolve as soon as possible as need to contact supplier regularly.
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>ticketCreator</t>
   </si>
@@ -65,24 +90,12 @@
     <t>solutionId3</t>
   </si>
   <si>
-    <t>Hier steht die Ticketnummer</t>
-  </si>
-  <si>
-    <t>Hier steht der Ticketersteller</t>
-  </si>
-  <si>
     <t>systemId</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>[{"start":3, "end":6, "key":"Fehlerbeschreibung"},{"start":45, "end":60, "key":"System"}]</t>
-  </si>
-  <si>
-    <t>Danke für deine Teilnahme</t>
-  </si>
-  <si>
     <t>01.12.2022</t>
   </si>
   <si>
@@ -92,9 +105,6 @@
     <t>Lisa Schmidt</t>
   </si>
   <si>
-    <t>Lukas Meyer</t>
-  </si>
-  <si>
     <t>Add-In "Analysis for Excel" verursacht Abstürze.</t>
   </si>
   <si>
@@ -104,24 +114,6 @@
     <t>17.01.2023</t>
   </si>
   <si>
-    <t>10.01.2023</t>
-  </si>
-  <si>
-    <t>Viele unserer Mitarbeiter nutzen "Analysis for Excel O365PP" - die meisten von ihnen erhalten eine Fehlermeldung und das Add-in wird nicht gestartet. Ich kann das Add-in manuell starten, aber nach einem Neustart (oder Excel-Neustart) ist das Add-in wieder inaktiv. Haben Sie eine Idee, was wir in diesem Fall tun können? Vielen Dank für Ihre Unterstützung.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installation Viseo 2016 Standard </t>
-  </si>
-  <si>
-    <t>Ich möchte Viseo 2016 Standard auf diesem Gerät installieren.</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Viele unserer Mitarbeiter nutzen &lt;a href="www.youtube.de" &gt;"Analysis for Excel O365PP"&lt;/a&gt; - die meisten von ihnen erhalten eine Fehlermeldung und das Add-in wird nicht gestartet. Ich kann das Add-in manuell starten, aber nach einem Neustart (oder Excel-Neustart) ist das Add-in wieder inaktiv. Haben Sie eine Idee, was wir in diesem Fall tun können? Vielen Dank für Ihre Unterstützung.</t>
-  </si>
-  <si>
     <t>pre_solutionId1</t>
   </si>
   <si>
@@ -129,13 +121,59 @@
   </si>
   <si>
     <t>pre_solutionId3</t>
+  </si>
+  <si>
+    <t>Karen Werner</t>
+  </si>
+  <si>
+    <t>Cisco Softphone funktioniert nicht</t>
+  </si>
+  <si>
+    <t>Campus 1 : MY / Cisco Softphone kann nicht verwendet werden
+2023-01-24 05:03:58 - Nutzer (Weitere Kommentare)
+Betroffenes Gerät: Cisco-Softphone
+Beschreibung des Problems: Das CISCO Softphone kann nicht verwendet werden, obwohl es vom IT-Support-Team installiert, eingerichtet und getestet wurde.
+Das Problem mit dem Softphone muss so schnell wie möglich gelöst werden, da wir den Lieferanten regelmäßig kontaktieren müssen.</t>
+  </si>
+  <si>
+    <t>Heinz Schubert</t>
+  </si>
+  <si>
+    <t>08.01.2023</t>
+  </si>
+  <si>
+    <t>Installation Nuance Software</t>
+  </si>
+  <si>
+    <t>Installation der Nuance PDF Software kann auf dem Laptop nicht gefunden werden.
+2023-01-08 12:08:29 - Nutzer (Weitere Kommentare)
+Muss ich mit dem VPN verbunden sein? Das Paket wird immer noch nicht im Portal Manager angezeigt. Die Checkpoint-App zur direkten Verbindung mit dem Braun-Netzwerk ist seit letzter Woche nicht mehr verfügbar.
+2023-01-08 10:04:06 - Nutzer (Weitere Kommentare)
+Die Anwendung wird im Portalmanager nicht gefunden.
+2023-01-07 16:25:56 - Nutzer (Weitere Kommentare)
+Zusätzliche Standortinformationen: 
+Betroffenes Gerät: ED12-D1234
+Beschreibung des Problems: Nuance-Software wurde über den IT-Shop bestellt und genehmigt. Die Anwendung kann jedoch im Portal Manager nicht zur Installation gefunden werden.</t>
+  </si>
+  <si>
+    <t>Vielen Dank für Ihre Teilnahme!</t>
+  </si>
+  <si>
+    <t>Bitte füllen Sie im Anschluss nun folgende &lt;a href="https://forms.gle/QxKwBcwiMtDbRGhd6" &gt;"Umfrage"&lt;/a&gt; aus. Im Anschluss würden wir Sie bitten an einem kurzen Interview teilzunehmen. Falls Sie noch keinen Termin haben sollten, kommen Sie hier zur &lt;a href="https://calendly.com/philipp-reinhard-1/interview_experiment" &gt;"Terminbuchung"&lt;/a&gt; .
+Vielen Dank, dass Sie unsere Forschung im Bereich künstlicher Intelligenz unterstützen!</t>
+  </si>
+  <si>
+    <t>05.01.2023</t>
+  </si>
+  <si>
+    <t>Ende des Experiments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,13 +181,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,14 +214,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -272,11 +375,17 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mike Mardari" id="{1920BDAA-5573-4ADE-9524-9D97B34FD187}" userId="ef6abb53d3923e8c" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}" name="Table2" displayName="Table2" ref="A1:M5" totalsRowShown="0">
   <autoFilter ref="A1:M5" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}"/>
   <tableColumns count="13">
-    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(A1+1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{F788B06C-E20D-499B-82A2-16BDBA4E08F2}" name="ticketId"/>
@@ -557,28 +666,43 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F3" dT="2023-01-02T19:43:13.37" personId="{1920BDAA-5573-4ADE-9524-9D97B34FD187}" id="{76F8C2AA-920B-4DF9-9FF9-807CFE50611C}">
+    <text xml:space="preserve">Hier Ende der Problembeschreobung weggelassen, da nicht verstanden, was gemeint ist.
+Original: Campus 1 : MY / Cisco soft phone unable to use
+2021-06-24 05:03:58 - Mas Azra Zabirah Mohd Azahari (Additional comments)
+Additional Location Information: 
+Affected Device: Cisco soft phone
+Issue description: Unable to use CISCO soft phone even though has been installed, set up and test by IT support team and no CISCO soft phone install in CITRIX in case  need to use the soft phone in the CITRIX window.
+Need soft phone issue to resolve as soon as possible as need to contact supplier regularly.
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" customWidth="1"/>
-    <col min="6" max="6" width="131.42578125" customWidth="1"/>
-    <col min="7" max="7" width="83.5703125" customWidth="1"/>
+    <col min="2" max="3" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="40.453125" customWidth="1"/>
+    <col min="6" max="6" width="131.453125" customWidth="1"/>
+    <col min="7" max="7" width="83.54296875" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="11" width="13.140625" customWidth="1"/>
+    <col min="9" max="11" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -608,248 +732,244 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
-        <f t="shared" ref="A2:A4" si="0">IFERROR(A1+1,0)</f>
+        <f t="shared" ref="A2" si="0">IFERROR(A1+1,0)</f>
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
+      <c r="B2">
+        <v>56011</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f>IFERROR(A2+1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>56012</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3" s="3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f>IFERROR(A2+1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>56013</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3">
+        <v>11</v>
+      </c>
+      <c r="I4">
         <v>13</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>15</v>
+      </c>
+      <c r="M4">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>123</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>456</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>IFERROR(A4+1,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
         <v>27</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:D4 G4:J4 A2:J3">
-    <cfRule type="containsBlanks" dxfId="12" priority="17">
+  <conditionalFormatting sqref="H2:J4">
+    <cfRule type="containsBlanks" dxfId="19" priority="24">
+      <formula>LEN(TRIM(H2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:J3">
+    <cfRule type="containsBlanks" dxfId="18" priority="23">
+      <formula>LEN(TRIM(H3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:J4">
+    <cfRule type="containsBlanks" dxfId="17" priority="22">
+      <formula>LEN(TRIM(H4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:F5">
+    <cfRule type="containsBlanks" dxfId="11" priority="11">
+      <formula>LEN(TRIM(E5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsBlanks" dxfId="8" priority="8">
+      <formula>LEN(TRIM(F5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:G2 A3:B3 G3 A4:C4 E4:G4 D3:D5">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:J3">
-    <cfRule type="containsBlanks" dxfId="11" priority="16">
-      <formula>LEN(TRIM(A3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:D4 G4:J4">
-    <cfRule type="containsBlanks" dxfId="10" priority="15">
-      <formula>LEN(TRIM(A4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="9" priority="13">
+  <conditionalFormatting sqref="B2:G2 B3 G3 A4:C4 E4:G4 D3:D5">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="containsBlanks" dxfId="8" priority="11">
-      <formula>LEN(TRIM(D4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
-      <formula>LEN(TRIM(D2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
-      <formula>LEN(TRIM(D2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
-      <formula>LEN(TRIM(F2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:F5">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
-      <formula>LEN(TRIM(D5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(D5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
-      <formula>LEN(TRIM(D5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(F5))=0</formula>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F3">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(E3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F3">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(E3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to be committed: modified:   client/public/wizard_of_oz_experiment_data_open.xlsx
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wikassel-my.sharepoint.com/personal/mahei_li_wi-kassel_de/Documents/Crowdsupport/05 Publikationen/2023/DESRIST_Reference Process for Labeling/03_Data Experiment/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF08C376-65BE-4F83-A5FD-670FE634A835}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5690DA5-E878-4A7E-808F-AB6D54346CF1}"/>
   <bookViews>
-    <workbookView xWindow="30936" yWindow="2640" windowWidth="30960" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openTickets" sheetId="1" r:id="rId1"/>
@@ -173,19 +173,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -225,65 +219,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -385,7 +323,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}" name="Table2" displayName="Table2" ref="A1:M5" totalsRowShown="0">
   <autoFilter ref="A1:M5" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}"/>
   <tableColumns count="13">
-    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(A1+1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{F788B06C-E20D-499B-82A2-16BDBA4E08F2}" name="ticketId"/>
@@ -685,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,8 +765,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f>IFERROR(A2+1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>56013</v>
@@ -869,8 +806,7 @@
     </row>
     <row r="5" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f>IFERROR(A4+1,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -911,27 +847,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:J4">
-    <cfRule type="containsBlanks" dxfId="19" priority="24">
+    <cfRule type="containsBlanks" dxfId="11" priority="24">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:J3">
-    <cfRule type="containsBlanks" dxfId="18" priority="23">
+    <cfRule type="containsBlanks" dxfId="10" priority="23">
       <formula>LEN(TRIM(H3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J4">
-    <cfRule type="containsBlanks" dxfId="17" priority="22">
+    <cfRule type="containsBlanks" dxfId="9" priority="22">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:F5">
-    <cfRule type="containsBlanks" dxfId="11" priority="11">
+    <cfRule type="containsBlanks" dxfId="8" priority="11">
       <formula>LEN(TRIM(E5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -961,7 +897,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   client/public/wizard_of_oz_experiment_data_open.xlsx 	modified:   client/public/wizard_of_oz_experiment_data_solution.xlsx
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wikassel-my.sharepoint.com/personal/mahei_li_wi-kassel_de/Documents/Crowdsupport/05 Publikationen/2023/DESRIST_Reference Process for Labeling/03_Data Experiment/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5690DA5-E878-4A7E-808F-AB6D54346CF1}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C32462A-E3E3-4FEC-8FDB-73AE14662E6B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24144" yWindow="2112" windowWidth="30936" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openTickets" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>ticketCreator</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>01.12.2022</t>
-  </si>
-  <si>
-    <t>[{"start":45, "end":60, "key":"Fehlerbeschreibung"},{"start":30, "end":45, "key":"System"}]</t>
   </si>
   <si>
     <t>Lisa Schmidt</t>
@@ -145,28 +142,31 @@
     <t>Installation Nuance Software</t>
   </si>
   <si>
+    <t>Vielen Dank für Ihre Teilnahme!</t>
+  </si>
+  <si>
+    <t>Bitte füllen Sie im Anschluss nun folgende &lt;a href="https://forms.gle/QxKwBcwiMtDbRGhd6" &gt;"Umfrage"&lt;/a&gt; aus. Im Anschluss würden wir Sie bitten an einem kurzen Interview teilzunehmen. Falls Sie noch keinen Termin haben sollten, kommen Sie hier zur &lt;a href="https://calendly.com/philipp-reinhard-1/interview_experiment" &gt;"Terminbuchung"&lt;/a&gt; .
+Vielen Dank, dass Sie unsere Forschung im Bereich künstlicher Intelligenz unterstützen!</t>
+  </si>
+  <si>
+    <t>05.01.2023</t>
+  </si>
+  <si>
+    <t>Ende des Experiments</t>
+  </si>
+  <si>
+    <t>[{ start: 143, end: 147, key: "System" }​,{ start: 104, end: 128, key: "Fehlerbeschreibung" }​,{ start: 67, end: 77, key: "System" }]</t>
+  </si>
+  <si>
+    <t>[{ start: 229, end: 297, key: "Service Anfrage" },​{ start: 191, end: 192, key: "System" }​,{ start: 176, end: 191, key: "System" }​,{ start: 129, end: 144, key: "System" }]</t>
+  </si>
+  <si>
+    <t>[{ start: 130, end: 165, key: "Auslöser" }​,{ start: 37, end: 78, key: "Fehlerbeschreibung" },​{ start: 24, end: 36, key: "System" }]</t>
+  </si>
+  <si>
     <t>Installation der Nuance PDF Software kann auf dem Laptop nicht gefunden werden.
 2023-01-08 12:08:29 - Nutzer (Weitere Kommentare)
-Muss ich mit dem VPN verbunden sein? Das Paket wird immer noch nicht im Portal Manager angezeigt. Die Checkpoint-App zur direkten Verbindung mit dem Braun-Netzwerk ist seit letzter Woche nicht mehr verfügbar.
-2023-01-08 10:04:06 - Nutzer (Weitere Kommentare)
-Die Anwendung wird im Portalmanager nicht gefunden.
-2023-01-07 16:25:56 - Nutzer (Weitere Kommentare)
-Zusätzliche Standortinformationen: 
-Betroffenes Gerät: ED12-D1234
-Beschreibung des Problems: Nuance-Software wurde über den IT-Shop bestellt und genehmigt. Die Anwendung kann jedoch im Portal Manager nicht zur Installation gefunden werden.</t>
-  </si>
-  <si>
-    <t>Vielen Dank für Ihre Teilnahme!</t>
-  </si>
-  <si>
-    <t>Bitte füllen Sie im Anschluss nun folgende &lt;a href="https://forms.gle/QxKwBcwiMtDbRGhd6" &gt;"Umfrage"&lt;/a&gt; aus. Im Anschluss würden wir Sie bitten an einem kurzen Interview teilzunehmen. Falls Sie noch keinen Termin haben sollten, kommen Sie hier zur &lt;a href="https://calendly.com/philipp-reinhard-1/interview_experiment" &gt;"Terminbuchung"&lt;/a&gt; .
-Vielen Dank, dass Sie unsere Forschung im Bereich künstlicher Intelligenz unterstützen!</t>
-  </si>
-  <si>
-    <t>05.01.2023</t>
-  </si>
-  <si>
-    <t>Ende des Experiments</t>
+Muss ich mit dem VPN verbunden sein? Das Paket wird immer noch nicht im Portal Manager angezeigt. Die Checkpoint-App zur direkten Verbindung mit dem Firmen-Netzwerk ist seit letzter Woche nicht mehr verfügbar.</t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,13 +670,13 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -688,19 +688,19 @@
         <v>56011</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -730,19 +730,19 @@
         <v>56012</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H3">
         <v>7</v>
@@ -763,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -771,19 +771,19 @@
         <v>56013</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
+      <c r="F4" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3">
         <v>11</v>
@@ -812,37 +812,37 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
       <c r="H5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="M5">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   client/public/wizard_of_oz_experiment_data_open.xlsx 	modified:   client/src/components/description.js
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wikassel-my.sharepoint.com/personal/mahei_li_wi-kassel_de/Documents/Crowdsupport/05 Publikationen/2023/DESRIST_Reference Process for Labeling/03_Data Experiment/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29D5865-E11E-46E5-A20C-F5239E7F9628}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{BB31B439-41D6-43DA-A261-F6A12F936545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55202B7E-C5D3-49AC-BBF5-BA9785EB4E18}"/>
   <bookViews>
-    <workbookView xWindow="24240" yWindow="8196" windowWidth="30936" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24144" yWindow="2112" windowWidth="30936" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openTickets" sheetId="1" r:id="rId1"/>
@@ -160,13 +160,13 @@
 Muss ich mit dem VPN verbunden sein? Das Paket wird immer noch nicht im Portal Manager angezeigt. Die Checkpoint-App zur direkten Verbindung mit dem Firmen-Netzwerk ist seit letzter Woche nicht mehr verfügbar.</t>
   </si>
   <si>
-    <t>[{" start": 143, "end": 147, "key": "System" }​,{ "start": 104, "end": 128, "key": "Fehlerbeschreibung" }​,{ "start": 67,"end": 77, "key": "System" }]</t>
-  </si>
-  <si>
     <t>[{"start": 229, "end": 297,"key": "Service Anfrage" },​{ "start": 191,"end": 192,"key": "System" }​,{"start": 176, "end": 191, "key": "System" }​,{"start": 129, "end": 144, "key": "System" }]</t>
   </si>
   <si>
     <t>[{"start": 130, "end": 165, "key": "Auslöser" }​,{ "start": 37, "end": 78, "key": "Fehlerbeschreibung" },​{ "start": 24, "end": 36, "key": "System" }]</t>
+  </si>
+  <si>
+    <t>[{"start": 143, "end": 147, "key": "System" }​,{ "start": 104, "end": 128, "key": "Fehlerbeschreibung" }​,{ "start": 67,"end": 77, "key": "System" }]</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -742,7 +742,7 @@
         <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3">
         <v>7</v>
@@ -783,7 +783,7 @@
         <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3">
         <v>11</v>

</xml_diff>

<commit_message>
modified:   README.md 	new file:   client/public/wizard_of_oz_experiment_data_open - Kopie.xlsx 	modified:   client/public/wizard_of_oz_experiment_data_open.xlsx 	new file:   client/public/wizard_of_oz_experiment_data_solution - Kopie.xlsx 	modified:   client/public/wizard_of_oz_experiment_data_solution.xlsx
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wikassel-my.sharepoint.com/personal/mahei_li_wi-kassel_de/Documents/Crowdsupport/05 Publikationen/2023/DESRIST_Reference Process for Labeling/03_Data Experiment/v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhilippReinhard\bandit-wizard-of-oz\wizard-of-oz\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F9D82C18-5952-4822-8835-9E8FB78AC67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F26D29-2614-4C9D-9BC1-D000C6A218B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44400" yWindow="3168" windowWidth="14400" windowHeight="7272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openTickets" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Lisa Schmidt</t>
   </si>
   <si>
-    <t>Add-In "Analysis for Excel" verursacht Abstürze.</t>
-  </si>
-  <si>
     <t>Hallo, gibt es eine stabilere Version von "Analysis for Excel" für Office 365? Diese Version verursacht eine Menge von Abstürzen, wenn sie mit VBA ausgeführt wird. Meine aktuelle Version ist 2.8.</t>
   </si>
   <si>
@@ -98,23 +95,10 @@
     <t>Karen Werner</t>
   </si>
   <si>
-    <t>Cisco Softphone funktioniert nicht</t>
-  </si>
-  <si>
     <t>Heinz Schubert</t>
   </si>
   <si>
     <t>08.01.2023</t>
-  </si>
-  <si>
-    <t>Installation Nuance Software</t>
-  </si>
-  <si>
-    <t>Vielen Dank für Ihre Teilnahme!</t>
-  </si>
-  <si>
-    <t>Bitte füllen Sie im Anschluss nun folgende &lt;a href="https://forms.gle/QxKwBcwiMtDbRGhd6" &gt;"Umfrage"&lt;/a&gt; aus. Im Anschluss würden wir Sie bitten an einem kurzen Interview teilzunehmen. Falls Sie noch keinen Termin haben sollten, kommen Sie hier zur &lt;a href="https://calendly.com/philipp-reinhard-1/interview_experiment" &gt;"Terminbuchung"&lt;/a&gt; .
-Vielen Dank, dass Sie unsere Forschung im Bereich künstlicher Intelligenz unterstützen!</t>
   </si>
   <si>
     <t>05.01.2023</t>
@@ -194,6 +178,21 @@
 2023-01-24 05:03:58 - Nutzer (Weitere Kommentare)
 Betroffenes Gerät: Cisco-Softphone
 Beschreibung des Problems: Das CISCO Softphone kann nicht verwendet werden, obwohl es vom IT-Support-Team installiert, eingerichtet und getestet wurde.</t>
+  </si>
+  <si>
+    <t>Analysis for Excel" add-in causes crashes.</t>
+  </si>
+  <si>
+    <t>Cisco Softphone does not work</t>
+  </si>
+  <si>
+    <t>Installing Nuance Software</t>
+  </si>
+  <si>
+    <t>Thank you for your participation!</t>
+  </si>
+  <si>
+    <t>Thank you for supporting our research in artificial intelligence!"</t>
   </si>
 </sst>
 </file>
@@ -246,10 +245,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -307,25 +303,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -344,7 +322,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}" name="Table2" displayName="Table2" ref="A1:M5" totalsRowShown="0">
   <autoFilter ref="A1:M5" xr:uid="{7064B924-F2FC-46C3-B05D-DC079E3D2967}"/>
   <tableColumns count="13">
-    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{A0CEA7F4-0404-4037-9E1B-1E5A093D521D}" name="systemId" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(A1+1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{F788B06C-E20D-499B-82A2-16BDBA4E08F2}" name="ticketId"/>
@@ -629,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,13 +654,13 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -697,16 +675,16 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -736,19 +714,19 @@
         <v>56012</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="H3">
         <v>7</v>
@@ -777,19 +755,19 @@
         <v>56013</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H4" s="3">
         <v>11</v>
@@ -810,7 +788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -818,16 +796,16 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -852,59 +830,44 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:J4">
-    <cfRule type="containsBlanks" dxfId="11" priority="24">
-      <formula>LEN(TRIM(H2))=0</formula>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
+      <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:J3">
-    <cfRule type="containsBlanks" dxfId="10" priority="23">
-      <formula>LEN(TRIM(H3))=0</formula>
+  <conditionalFormatting sqref="A2:G2 A3:B3">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:J4">
-    <cfRule type="containsBlanks" dxfId="9" priority="22">
-      <formula>LEN(TRIM(H4))=0</formula>
+  <conditionalFormatting sqref="B3:B4">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(B3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G2 G3 D3:D5 A4:C4 E4:G4">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:F5">
-    <cfRule type="containsBlanks" dxfId="8" priority="11">
+    <cfRule type="containsBlanks" dxfId="2" priority="11">
       <formula>LEN(TRIM(E5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+    <cfRule type="containsBlanks" dxfId="1" priority="8">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G2 A3:B3 G3 A4:C4 E4:G4 D3:D5">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G2 B3 G3 A4:C4 E4:G4 D3:D5">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F3">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(E3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F3">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(E3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(B4))=0</formula>
+  <conditionalFormatting sqref="H2:J4">
+    <cfRule type="containsBlanks" dxfId="0" priority="22">
+      <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified:   client/public/wizard_of_oz_experiment_data_open.xlsx 	modified:   client/src/App.js
</commit_message>
<xml_diff>
--- a/client/public/wizard_of_oz_experiment_data_open.xlsx
+++ b/client/public/wizard_of_oz_experiment_data_open.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhilippReinhard\bandit-wizard-of-oz\wizard-of-oz\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F0EBF3-9B55-4983-8AEC-9D2367F48911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61896CE-EC38-408A-8B0F-CD5FFAA7CB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,6 +104,35 @@
     <t>Ende des Experiments</t>
   </si>
   <si>
+    <t>Analysis for Excel" add-in causes crashes.</t>
+  </si>
+  <si>
+    <t>Cisco Softphone does not work</t>
+  </si>
+  <si>
+    <t>Installing Nuance Software</t>
+  </si>
+  <si>
+    <t>Thank you for your participation!</t>
+  </si>
+  <si>
+    <t>Thank you for supporting our research in artificial intelligence!"</t>
+  </si>
+  <si>
+    <t>Hello, is there a more stable version of "Analysis for Excel" for Office 365? This version causes a lot of crashes when run with VBA. My current version is 2.8.</t>
+  </si>
+  <si>
+    <t>Campus 1 : MY / Cisco softphone cannot be used
+2023-01-24 05:03:58 - User (More comments)
+Affected device: Cisco softphone
+Description of the problem: The CISCO softphone cannot be used even though it has been installed, set up and tested by the IT support team.</t>
+  </si>
+  <si>
+    <t>Nuance PDF software installation cannot be found on laptop.
+2023-01-08 12:08:29 - User (More Comments).
+Do I need to be connected to the VPN? The package is still not showing up in the Portal Manager. The Checkpoint app to connect directly to the corporate network has been unavailable since last week.</t>
+  </si>
+  <si>
     <t>[
    {
       "start":143,
@@ -113,7 +142,7 @@
    {
       "start":104,
       "end":128,
-      "key":"Fehlerbeschreibung"
+      "key":"Error description"
    },
    {
       "start":67,
@@ -127,12 +156,12 @@
    {
       "start":130,
       "end":165,
-      "key":"Auslöser"
+      "key":"Trigger"
    },
    {
       "start":37,
       "end":78,
-      "key":"Fehlerbeschreibung"
+      "key":"Error description"
    },
    {
       "start":24,
@@ -146,7 +175,7 @@
    {
       "start":229,
       "end":297,
-      "key":"Service Anfrage"
+      "key":"Service request"
    },
    {
       "start":191,
@@ -164,35 +193,6 @@
       "key":"System"
    }
 ]</t>
-  </si>
-  <si>
-    <t>Analysis for Excel" add-in causes crashes.</t>
-  </si>
-  <si>
-    <t>Cisco Softphone does not work</t>
-  </si>
-  <si>
-    <t>Installing Nuance Software</t>
-  </si>
-  <si>
-    <t>Thank you for your participation!</t>
-  </si>
-  <si>
-    <t>Thank you for supporting our research in artificial intelligence!"</t>
-  </si>
-  <si>
-    <t>Hello, is there a more stable version of "Analysis for Excel" for Office 365? This version causes a lot of crashes when run with VBA. My current version is 2.8.</t>
-  </si>
-  <si>
-    <t>Campus 1 : MY / Cisco softphone cannot be used
-2023-01-24 05:03:58 - User (More comments)
-Affected device: Cisco softphone
-Description of the problem: The CISCO softphone cannot be used even though it has been installed, set up and tested by the IT support team.</t>
-  </si>
-  <si>
-    <t>Nuance PDF software installation cannot be found on laptop.
-2023-01-08 12:08:29 - User (More Comments).
-Do I need to be connected to the VPN? The package is still not showing up in the Portal Manager. The Checkpoint app to connect directly to the corporate network has been unavailable since last week.</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,13 +678,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -720,13 +720,13 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="H3">
         <v>7</v>
@@ -761,13 +761,13 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3">
         <v>11</v>
@@ -802,10 +802,10 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>

</xml_diff>